<commit_message>
first version of analytical solution to tests 2 and 6 - matlab code in place for mizuroute
</commit_message>
<xml_diff>
--- a/4_nrTrans_contS_PorMedia/mizuroute/mizuroute_in/shapefile/Calc_lengths.xlsx
+++ b/4_nrTrans_contS_PorMedia/mizuroute/mizuroute_in/shapefile/Calc_lengths.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/diogocosta/Library/CloudStorage/OneDrive-impactblue-scientific.com/6_Projects/1_GWF/2_WIP/code/mizuRoute/case_studies/synthetic_tests/4_nrTrans_contS_PorMedia/mizuroute/mizuroute_in/shapefile/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{48072A3A-9BC7-824B-A656-B09679DAC1E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EA4F7D5-02DD-0F4B-9CB3-D4D930BDDD4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3580" yWindow="2160" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{CC6DB487-1A3B-7C49-8420-03B3B9902D67}"/>
+    <workbookView xWindow="3900" yWindow="4900" windowWidth="28040" windowHeight="17440" xr2:uid="{CC6DB487-1A3B-7C49-8420-03B3B9902D67}"/>
   </bookViews>
   <sheets>
     <sheet name="Length_1" sheetId="1" r:id="rId1"/>
@@ -1529,14 +1529,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{144D415B-2464-5C4B-A53C-2A5718F94132}">
-  <dimension ref="C4:T101"/>
+  <dimension ref="C2:T97"/>
   <sheetViews>
-    <sheetView topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="I101" sqref="I101"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="11" max="11" width="15.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
+    <row r="2" spans="3:20" x14ac:dyDescent="0.2">
+      <c r="I2" s="2">
+        <f>SUM(I5:I97)</f>
+        <v>80.347999999999999</v>
+      </c>
+      <c r="O2" s="2">
+        <f>SUM(O5:O97)</f>
+        <v>0.83213459492728103</v>
+      </c>
+    </row>
     <row r="4" spans="3:20" x14ac:dyDescent="0.2">
       <c r="C4" t="s">
         <v>0</v>
@@ -6745,12 +6758,6 @@
       </c>
       <c r="T97">
         <v>1642.5620999999801</v>
-      </c>
-    </row>
-    <row r="101" spans="3:20" x14ac:dyDescent="0.2">
-      <c r="I101" s="2">
-        <f>SUM(I5:I97)</f>
-        <v>80.347999999999999</v>
       </c>
     </row>
   </sheetData>
@@ -13949,7 +13956,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7416E75-C476-2843-BCEA-92C7787D334D}">
   <dimension ref="B3:S130"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>

</xml_diff>